<commit_message>
FIX: Handling DB search error
</commit_message>
<xml_diff>
--- a/datasets/lyrics_data.xlsx
+++ b/datasets/lyrics_data.xlsx
@@ -466,73 +466,58 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>"I Will Follow" lyrics</t>
+          <t>"Fight Fire With Fire" lyrics</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>I will follow
-I was on the outside
-When you said, you said you needed me
-And I was looking at myself
-I was blind, I could not see
-A boy tries hard to be a man
-His mother takes him by his hand
-If he stops to think, he starts to cry
-Oh, why?
-If you walk away, walk away
-I walk away, walk away
-I will follow
-If you walk away, walk away
-I walk away, walk away
-I will follow
-I will follow
-I was on the inside
-When they pulled the four walls down
-I was looking through the window
-I was lost, I am found
-Walk away, walk away
-I walk away, walk away
-I will follow
-If you walk away, walk away
-I walk away, walk away
-I will follow
-I will follow
-Your eyes make a circle
-I see you when I go in there
-Your eyes
-Your, your, your eyes
-Your eyes, just give me
-Your, your, your eyes
-Mmm, mmm, mmm, mmm
-If you walk away, walk away
-I walk away, walk away
-I will follow
-If you walk away, walk away
-I walk away, walk away
-I will follow
-I will follow
-I will follow
-I will follow
-I will follow
-Follow</t>
+          <t>Do unto others as they've done to you
+But what the hell is this world coming to?
+Blow the universe into nothingness
+Nuclear warfare shall lay us to rest
+Fight fire with fire
+Ending is near
+Fight fire with fire
+Bursting with fear
+We all shall die
+Time is like a fuse, short and burning fast
+Armageddon's here, like said in the past
+Fight fire with fire
+Ending is near
+Fight fire with fire
+Bursting with fear
+Soon to fill our lungs, the hot winds of death
+The gods are laughing, so take your last breath
+Fight fire with fire
+Ending is near
+Fight fire with fire
+Bursting with fear
+Fight fire with fire
+Fight fire with fire
+Fight fire with fire
+Fight fire with fire
+Fight fire with fire
+Fight fire with fire
+Fight fire with fire
+Fight fire with fire
+Fight</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
           <t xml:space="preserve">
-U2 Lyrics
+Metallica Lyrics
 </t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>album: "Boy" (1980)</t>
+          <t>album: "Ride The Lightning" (1984)</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Submit CorrectionsWriter(s): Adam Clayton, Larry Mullen, Dave Evans, Paul David Hewson</t>
+          <t>Submit CorrectionsThanks to Grenas for correcting these lyrics.Writer(s): Lars Ulrich, James Alan Hetfield, Clifford Lee Burton</t>
         </is>
       </c>
     </row>
@@ -542,75 +527,68 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>"The Electric Co." lyrics</t>
+          <t>"One" lyrics</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Boy, stupid boy
-Don't sit at the table
-Until you're able to
-Toy, broken toy
-Shout, shout, you're inside out
-If you don't know
-Electric Co
-If you don't know
-Electric Co
-Red, running red
-Play for real
-Talk and feel
-A hole in your head
-You won't shout
-You're spoon fed
-If you don't know
-Electric Co
-If you don't know
-Electric Co
-Two, three, four
-I can't stop
-Useless is the castle wall
-Useless is the metal wall
-He's gonna jump
-If you don't know
-Electric Co
-If you don't know
-Electric Co
-If you don't know
-Electric Co
-If you don't know
-Electric Co
-If you don't know
-Electric Co
-If you don't know
-Electric Co
-Till someone leaves him below
-He's searched high and low
-A tap on the wrist and he'd know
-Somebody hear him
-Just leave him
-I can't find my way home
-I'm alone
-I've lost my way home
-You know and you know
-And you know and you know
-And you know</t>
+          <t>I can't remember anything
+Can't tell if this is true or dream
+Deep down inside I feel the scream
+This terrible silence stops me
+Now that the war is through with me
+I'm waking up, I cannot see
+That there's not much left of me
+Nothing is real but pain now
+Hold my breath as I wish for death
+Oh please, God, wake me
+Back in the womb it's much too real
+In pumps life that I must feel
+But can't look forward to reveal
+Look to the time when I'll live
+Fed through the tube that sticks in me
+Just like a wartime novelty
+Tied to machines that make me be
+Cut this life off from me
+Hold my breath as I wish for death
+Oh please, God, wake me
+Now the world is gone, I'm just one
+Oh God, help me
+Hold my breath as I wish for death
+Oh please, God, help me
+Darkness
+Imprisoning me
+All that I see
+Absolute horror
+I cannot live
+I cannot die
+Trapped in myself
+Body my holding cell
+Landmine
+Has taken my sight
+Taken my speech
+Taken my hearing
+Taken my arms
+Taken my legs
+Taken my soul
+Left me with life in hell</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
           <t xml:space="preserve">
-U2 Lyrics
+Metallica Lyrics
 </t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>album: "Boy" (1980)</t>
+          <t>album: "...And Justice For All" (1988)</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Submit CorrectionsWriter(s): Larry Mullen, Paul David Hewson, Adam Clayton, Dave Evans, Brian Peter George Eno</t>
+          <t>Submit CorrectionsThanks to Payton for correcting these lyrics.Writer(s): Lars Ulrich, James Alan Hetfield</t>
         </is>
       </c>
     </row>
@@ -620,62 +598,84 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>"Twilight" lyrics</t>
+          <t>"Fuel" lyrics</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>I look into his eyes
-They're closed but I see something
-A teacher told me why
-I laugh when old men cry
-My body grows and grows
-It frightens me you know
-The old man tried to walk me home
-I thought he should have known
-Twilight...
-Twilight, lost my way
-Twilight, can't find my way
-In the shadow boy meets man
-In the shadow boy meets man
-In the shadow boy meets man
-In the shadow boy meets man
-I'm running in the rain
-I'm caught in a late night play
-It's all; it's everything
-I'm soaking through the skin
-Twilight...darkened day
-Twilight...lost my way
-Twilight...night and day
-Twilight...can't find my way
-Can't find your way
-Can't find my way
-Can't find your way
-Twilight...darkened day
-Twilight...lost my way
-Twilight...night and day
-Twilight...can't find my way
-In the shadow boy meets man
-In the shadow boy meets man
-In the shadow boy meets man
-In the shadow boy meets man</t>
+          <t>Gimme fuel
+Gimme fire
+Gimme that which I desire
+Ooh!
+Yeah!
+Turn on... I see red
+Adrenaline crash and crack my head
+Nitro junkie, paint me dead
+And I see red
+One hundred plus through black and white
+War horse, warhead
+Fuck 'em man, white-knuckle tight
+Through black and white
+On I burn
+Fuel is pumping engines
+Burning hard, loose and clean
+And on I burn
+Churning my direction
+Quench my thirst with gasoline
+So gimme fuel
+Gimme fire
+Gimme that which I desire
+Ooh
+Turn on beyond the bone
+Swallow future, spit out home
+Burn your face upon the chrome
+Yeah!
+Take the corner, join the crash
+Headlights, head on, headlines
+Another junkie lives too fast
+Yeah lives way too fast, fast, fast, oohhOH!
+On I burn
+Fuel is pumping engines
+Burning hard, loose and clean
+And on I burn
+Churning my direction
+Quench my thirst with gasoline
+So gimme fuel
+Gimme fire
+Gimme that which I desire
+Yeah-heah
+White knuckle tight!
+Gimme fuel
+Gimme fire
+My desire
+On I burn
+Fuel is pumping engines
+Burning hard, loose and clean
+And on I burn
+Churning my direction
+Quench my thirst with gasoline
+Gimme fuel
+Gimme fire
+Gimme that which I desire
+Ooh
+On I burn</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
           <t xml:space="preserve">
-U2 Lyrics
+Metallica Lyrics
 </t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>album: "Boy" (1980)</t>
+          <t>album: "Reload" (1997)</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Submit Corrections</t>
+          <t>Submit CorrectionsThanks to chloe for correcting these lyrics.Writer(s): Eliot Kennedy, Bryan Adams</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added DB Wrangling Script
</commit_message>
<xml_diff>
--- a/datasets/lyrics_data.xlsx
+++ b/datasets/lyrics_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,216 +466,48 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>"Fight Fire With Fire" lyrics</t>
+          <t>"Dont Panic" lyrics</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Do unto others as they've done to you
-But what the hell is this world coming to?
-Blow the universe into nothingness
-Nuclear warfare shall lay us to rest
-Fight fire with fire
-Ending is near
-Fight fire with fire
-Bursting with fear
-We all shall die
-Time is like a fuse, short and burning fast
-Armageddon's here, like said in the past
-Fight fire with fire
-Ending is near
-Fight fire with fire
-Bursting with fear
-Soon to fill our lungs, the hot winds of death
-The gods are laughing, so take your last breath
-Fight fire with fire
-Ending is near
-Fight fire with fire
-Bursting with fear
-Fight fire with fire
-Fight fire with fire
-Fight fire with fire
-Fight fire with fire
-Fight fire with fire
-Fight fire with fire
-Fight fire with fire
-Fight fire with fire
-Fight</t>
+          <t>Bones sinking like stones
+All that we fought for
+Homes, places we've grown
+All of us are done for
+And we live in a beautiful world
+Yeah we do, yeah we do
+We live in a beautiful world
+Bones sinking like stones
+All that we fought for
+And homes, places we've grown
+All of us are done for
+And we live in a beautiful world
+Yeah we do, yeah we do
+We live in a beautiful world
+And we live in a beautiful world
+Yeah we do, yeah we do
+We live in a beautiful world
+Oh, all that I know
+There's nothing here to run from
+'Cause yeah everybody here's got somebody to lean on</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
           <t xml:space="preserve">
-Metallica Lyrics
+Coldplay Lyrics
 </t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>album: "Ride The Lightning" (1984)</t>
+          <t>EP: "The Blue Room" (1999)</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Submit CorrectionsThanks to Grenas for correcting these lyrics.Writer(s): Lars Ulrich, James Alan Hetfield, Clifford Lee Burton</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>"One" lyrics</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>I can't remember anything
-Can't tell if this is true or dream
-Deep down inside I feel the scream
-This terrible silence stops me
-Now that the war is through with me
-I'm waking up, I cannot see
-That there's not much left of me
-Nothing is real but pain now
-Hold my breath as I wish for death
-Oh please, God, wake me
-Back in the womb it's much too real
-In pumps life that I must feel
-But can't look forward to reveal
-Look to the time when I'll live
-Fed through the tube that sticks in me
-Just like a wartime novelty
-Tied to machines that make me be
-Cut this life off from me
-Hold my breath as I wish for death
-Oh please, God, wake me
-Now the world is gone, I'm just one
-Oh God, help me
-Hold my breath as I wish for death
-Oh please, God, help me
-Darkness
-Imprisoning me
-All that I see
-Absolute horror
-I cannot live
-I cannot die
-Trapped in myself
-Body my holding cell
-Landmine
-Has taken my sight
-Taken my speech
-Taken my hearing
-Taken my arms
-Taken my legs
-Taken my soul
-Left me with life in hell</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-Metallica Lyrics
-</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>album: "...And Justice For All" (1988)</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Submit CorrectionsThanks to Payton for correcting these lyrics.Writer(s): Lars Ulrich, James Alan Hetfield</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>"Fuel" lyrics</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Gimme fuel
-Gimme fire
-Gimme that which I desire
-Ooh!
-Yeah!
-Turn on... I see red
-Adrenaline crash and crack my head
-Nitro junkie, paint me dead
-And I see red
-One hundred plus through black and white
-War horse, warhead
-Fuck 'em man, white-knuckle tight
-Through black and white
-On I burn
-Fuel is pumping engines
-Burning hard, loose and clean
-And on I burn
-Churning my direction
-Quench my thirst with gasoline
-So gimme fuel
-Gimme fire
-Gimme that which I desire
-Ooh
-Turn on beyond the bone
-Swallow future, spit out home
-Burn your face upon the chrome
-Yeah!
-Take the corner, join the crash
-Headlights, head on, headlines
-Another junkie lives too fast
-Yeah lives way too fast, fast, fast, oohhOH!
-On I burn
-Fuel is pumping engines
-Burning hard, loose and clean
-And on I burn
-Churning my direction
-Quench my thirst with gasoline
-So gimme fuel
-Gimme fire
-Gimme that which I desire
-Yeah-heah
-White knuckle tight!
-Gimme fuel
-Gimme fire
-My desire
-On I burn
-Fuel is pumping engines
-Burning hard, loose and clean
-And on I burn
-Churning my direction
-Quench my thirst with gasoline
-Gimme fuel
-Gimme fire
-Gimme that which I desire
-Ooh
-On I burn</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-Metallica Lyrics
-</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>album: "Reload" (1997)</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Submit CorrectionsThanks to chloe for correcting these lyrics.Writer(s): Eliot Kennedy, Bryan Adams</t>
+          <t>Submit CorrectionsWriter(s): Jonathan Mark Buckland, Christopher Anthony John Martin, William Champion, Guy Rupert Berryman</t>
         </is>
       </c>
     </row>

</xml_diff>